<commit_message>
the rest of hwk 9!
</commit_message>
<xml_diff>
--- a/2nd Half.xlsx
+++ b/2nd Half.xlsx
@@ -4,10 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dividends" sheetId="1" r:id="rId1"/>
+    <sheet name="Timeline" sheetId="2" r:id="rId2"/>
+    <sheet name="Equity" sheetId="3" r:id="rId3"/>
+    <sheet name="PE vs PB" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,15 +21,196 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
+  <si>
+    <t xml:space="preserve">Stock Price = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected Price = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equity Cost of Captial = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dividend = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Price = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dividen Yield = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capital Gain Rate = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dividend Growth Rate = </t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dividend Increase = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equity Cost of Capital = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Payout = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repurcahse Amount = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">g = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rE = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equity Value  = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Shares = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected FCF 2015 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enterprise Value 2014 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected FCF 2014 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enterprise Value 2013 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excess Cash 2013 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debt in 2013 = </t>
+  </si>
+  <si>
+    <t>P/E</t>
+  </si>
+  <si>
+    <t>Price/Book</t>
+  </si>
+  <si>
+    <t>Enterprise Value/Sales</t>
+  </si>
+  <si>
+    <t>enterprise Value/EBITDA</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share Price = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPS = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Book Equity = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year 0 Dividend = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year 1 Dividend = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual Dividend Groth Rate = </t>
+  </si>
+  <si>
+    <t>Dividen N</t>
+  </si>
+  <si>
+    <t>1st ()</t>
+  </si>
+  <si>
+    <t>2nd ()</t>
+  </si>
+  <si>
+    <t>3rd ()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dividend Year 0 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dividend Year 1 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PV first 5 years = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increase Year 1 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">After 5 years Growth Rate = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PV First 5 years = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FV Other Years = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">post years = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PV = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FV after x years = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PV after x years = </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF2D3639"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +221,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +229,77 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,12 +580,892 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1">
+        <v>1.26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>43.6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>13</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="20">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="22">
+        <f>H1*H2+H1</f>
+        <v>1.4484000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5">
+        <f>B2*(1+B3)-B1</f>
+        <v>45.915200000000006</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="9">
+        <f>(E3-E2)/E2</f>
+        <v>0.23076923076923078</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="23">
+        <v>8.3000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7">
+        <f>B1/B2</f>
+        <v>2.8899082568807338E-2</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="13">
+        <f>E1/E2</f>
+        <v>0.15384615384615385</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="24">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="13">
+        <f>E4+E5</f>
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="9">
+        <f>H4-(H3/H5)</f>
+        <v>4.8514285714285718E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <v>1.36</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>4.67</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="20">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="15">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="22">
+        <f>B8*B9+B8</f>
+        <v>1.4484000000000001</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="15"/>
+      <c r="G10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="29">
+        <f>1-H8/H9</f>
+        <v>7.4074074074074181E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="18">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="17">
+        <v>51.46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="21">
+        <f>B10/(B11-B9)</f>
+        <v>80.466666666666669</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="9">
+        <f>(E8/E11) + E9</f>
+        <v>0.11875009716284492</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="601" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="31">
+        <f>($B$12+$B$11*B1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="C2" s="31">
+        <f>B2+$B$11</f>
+        <v>1.62</v>
+      </c>
+      <c r="D2" s="31">
+        <f t="shared" ref="D2:I2" si="0">C2+$B$11</f>
+        <v>1.7400000000000002</v>
+      </c>
+      <c r="E2" s="31">
+        <f t="shared" si="0"/>
+        <v>1.8600000000000003</v>
+      </c>
+      <c r="F2" s="31">
+        <f t="shared" si="0"/>
+        <v>1.9800000000000004</v>
+      </c>
+      <c r="G2" s="31">
+        <f t="shared" si="0"/>
+        <v>2.1000000000000005</v>
+      </c>
+      <c r="H2" s="31">
+        <f t="shared" si="0"/>
+        <v>2.2200000000000006</v>
+      </c>
+      <c r="I2" s="31">
+        <f t="shared" si="0"/>
+        <v>2.3400000000000007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="5">
+        <f>B2/POWER(1+$B$9, B1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="C3" s="5">
+        <f t="shared" ref="C3:I3" si="1">C2/POWER(1+$B$9, C1)</f>
+        <v>1.4930875576036868</v>
+      </c>
+      <c r="D3" s="5">
+        <f t="shared" si="1"/>
+        <v>1.4780521990273738</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" si="1"/>
+        <v>1.4562090630811566</v>
+      </c>
+      <c r="F3" s="5">
+        <f t="shared" si="1"/>
+        <v>1.4287170828505478</v>
+      </c>
+      <c r="G3" s="5">
+        <f t="shared" si="1"/>
+        <v>1.3965953889057166</v>
+      </c>
+      <c r="H3" s="5">
+        <f t="shared" si="1"/>
+        <v>1.360738101106294</v>
+      </c>
+      <c r="I3" s="5">
+        <f t="shared" si="1"/>
+        <v>1.3219276608082067</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" s="5">
+        <f>SUM(B3:G3)</f>
+        <v>8.7526612914684812</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="5">
+        <f>1/POWER(1+$B$10, 5)</f>
+        <v>0.74725817286605689</v>
+      </c>
+      <c r="C4" s="5">
+        <f t="shared" ref="C4:I4" si="2">1/POWER(1+$B$10, 5)</f>
+        <v>0.74725817286605689</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" si="2"/>
+        <v>0.74725817286605689</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="2"/>
+        <v>0.74725817286605689</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" si="2"/>
+        <v>0.74725817286605689</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" si="2"/>
+        <v>0.74725817286605689</v>
+      </c>
+      <c r="H4" s="5">
+        <f t="shared" si="2"/>
+        <v>0.74725817286605689</v>
+      </c>
+      <c r="I4" s="5">
+        <f t="shared" si="2"/>
+        <v>0.74725817286605689</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="5">
+        <f>(B12*POWER(1+B16,5))/(1+B9-B10)</f>
+        <v>2.1502362099512204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="28">
+        <f>$H$2/($B$9-$B$10)</f>
+        <v>88.8</v>
+      </c>
+      <c r="C5" s="28">
+        <f t="shared" ref="C5:I5" si="3">$H$2/($B$9-$B$10)</f>
+        <v>88.8</v>
+      </c>
+      <c r="D5" s="28">
+        <f t="shared" si="3"/>
+        <v>88.8</v>
+      </c>
+      <c r="E5" s="28">
+        <f t="shared" si="3"/>
+        <v>88.8</v>
+      </c>
+      <c r="F5" s="28">
+        <f t="shared" si="3"/>
+        <v>88.8</v>
+      </c>
+      <c r="G5" s="28">
+        <f t="shared" si="3"/>
+        <v>88.8</v>
+      </c>
+      <c r="H5" s="3">
+        <f t="shared" si="3"/>
+        <v>88.8</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="3"/>
+        <v>88.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <f>B3+B4*B5</f>
+        <v>67.856525750505853</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" ref="C6:I6" si="4">C3+C4*C5</f>
+        <v>67.849613308109539</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="4"/>
+        <v>67.834577949533227</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="4"/>
+        <v>67.812734813587014</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="4"/>
+        <v>67.785242833356406</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="4"/>
+        <v>67.753121139411576</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="4"/>
+        <v>67.717263851612145</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="4"/>
+        <v>67.678453411314052</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="15">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9">
+        <f>B12*(1+B16)/(B9-B16)*(1-POWER((1+B16)/(1+B9),5))</f>
+        <v>7.3969482576469412</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10">
+        <f>((B12*POWER(1+B16, F14))/(1+B9-B16))*((1+B10)/(B9-B10))</f>
+        <v>193.91289771014712</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0.12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11">
+        <f>F10/POWER(1+B9, F14)</f>
+        <v>59.1703319409241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12">
+        <v>1.5</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12">
+        <f>F9+F11</f>
+        <v>66.567280198571041</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F13" s="32"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14">
+        <f>B12</f>
+        <v>1.5</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14">
+        <v>14.55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="3">
+        <f>B11</f>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="23">
+        <f>B15/B14</f>
+        <v>0.08</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="601" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1">
+        <v>2.84</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="20">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="15">
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="5">
+        <f>B1*(1+B2)</f>
+        <v>3.0274399999999999</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="20">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="21">
+        <f>E1/(E2-E3)</f>
+        <v>1018.5185185185185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="5">
+        <f>B3/(B4-B2)</f>
+        <v>201.82933333333332</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.436</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="5">
+        <f>(E4+E5)/(1+E2)</f>
+        <v>976.70796939535501</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5">
+        <f>B5/B6</f>
+        <v>462.91131498470946</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="5">
+        <f>E6+E7-E8</f>
+        <v>1049.7079693953551</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <f>E9/E10</f>
+        <v>20.994159387907104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="601" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>15.01</v>
+      </c>
+      <c r="C2">
+        <v>2.84</v>
+      </c>
+      <c r="D2">
+        <v>1.06</v>
+      </c>
+      <c r="E2">
+        <v>8.49</v>
+      </c>
+      <c r="F2">
+        <f>SUM(B2:E2)</f>
+        <v>27.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="19">
+        <v>0.51</v>
+      </c>
+      <c r="C3" s="19">
+        <v>1.86</v>
+      </c>
+      <c r="D3" s="19">
+        <v>1.06</v>
+      </c>
+      <c r="E3" s="19">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="19">
+        <v>-0.42</v>
+      </c>
+      <c r="C4" s="19">
+        <v>-0.61</v>
+      </c>
+      <c r="D4" s="19">
+        <v>-0.56000000000000005</v>
+      </c>
+      <c r="E4" s="19">
+        <v>-0.22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="5">
+        <f>B6*B2</f>
+        <v>28.218799999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="5">
+        <f>B7+(B7*B3)</f>
+        <v>42.610388</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="5">
+        <f>B7+(B7*B4)</f>
+        <v>16.366903999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="3">
+        <v>12.48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="5">
+        <f>B11*C2</f>
+        <v>35.443199999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="5">
+        <f>B12+(B12*C3)</f>
+        <v>101.36755199999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="5">
+        <f>B12+(B12*C4)</f>
+        <v>13.822848</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
a few more donw!
</commit_message>
<xml_diff>
--- a/2nd Half.xlsx
+++ b/2nd Half.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="81">
   <si>
     <t xml:space="preserve">Stock Price = </t>
   </si>
@@ -242,6 +242,30 @@
   </si>
   <si>
     <t>.b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected Return </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cash </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Borrow </t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volitility </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volatility </t>
+  </si>
+  <si>
+    <t xml:space="preserve">a. Sharpe Ratio </t>
   </si>
 </sst>
 </file>
@@ -304,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -368,6 +392,19 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1541,10 +1578,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1552,13 +1589,14 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" s="37" t="s">
         <v>58</v>
       </c>
@@ -1586,11 +1624,11 @@
       <c r="J1" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="K1" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -1627,12 +1665,12 @@
         <f>I2/$I$5</f>
         <v>0.3363317244405441</v>
       </c>
-      <c r="K2" s="35">
+      <c r="K2" s="43">
         <f>I2*D2/$I$5</f>
         <v>4.035980693286529</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1669,12 +1707,12 @@
         <f t="shared" ref="J3:J4" si="3">I3/$I$5</f>
         <v>0.20842474769635805</v>
       </c>
-      <c r="K3" s="35">
+      <c r="K3" s="43">
         <f t="shared" ref="K3:K4" si="4">I3*D3/$I$5</f>
         <v>2.0842474769635806</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -1711,12 +1749,12 @@
         <f t="shared" si="3"/>
         <v>0.45524352786309785</v>
       </c>
-      <c r="K4" s="36">
+      <c r="K4" s="44">
         <f t="shared" si="4"/>
         <v>3.6419482229047828</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E5" s="21">
         <f>SUM(E2:E4)</f>
         <v>914800</v>
@@ -1730,12 +1768,15 @@
         <v>911600</v>
       </c>
       <c r="J5" s="7"/>
-      <c r="K5" s="35">
+      <c r="K5" s="43">
         <f>SUM(K2:K4)</f>
         <v>9.7621763931548919</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G6" s="35"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>68</v>
       </c>
@@ -1745,56 +1786,141 @@
       <c r="D8" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E8" s="42"/>
+      <c r="G8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" s="19">
+        <v>0.13</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L8" s="15">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>66</v>
       </c>
       <c r="B9" s="15">
-        <v>7.0999999999999994E-2</v>
+        <v>0.12</v>
       </c>
       <c r="C9" s="15">
-        <v>0.16600000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="D9" s="19">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E9" s="41"/>
+      <c r="G9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="19">
+        <v>0.03</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L9" s="15">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>67</v>
       </c>
       <c r="B10" s="20">
-        <v>9.8000000000000004E-2</v>
+        <v>0.1</v>
       </c>
       <c r="C10" s="15">
-        <v>0.20100000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="D10" s="19">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E10" s="5"/>
+      <c r="G10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="19">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L10" s="20">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="9">
         <f>D9*B9+D10*B10</f>
-        <v>8.4499999999999992E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.11</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="L11" s="5">
+        <f>(L8-L10)/L9</f>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="38">
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>70</v>
       </c>
       <c r="B13" s="19">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" s="39">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>72</v>
       </c>
       <c r="B14" s="7">
         <f>SQRT(POWER(D9,2)*POWER(C9,2)+POWER(D10,2)*POWER(C10,2)+2*B13*D9*C9*D10*C10)</f>
-        <v>0.14373416434515493</v>
+        <v>0.1764227876437735</v>
+      </c>
+      <c r="G14" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14">
+        <f>(H12+H13)/H12</f>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G16" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="15">
+        <f>H9+H14*(H10-H9)</f>
+        <v>8.6000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G17" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="15">
+        <f>H8*H14</f>
+        <v>0.182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
half way through 26!
</commit_message>
<xml_diff>
--- a/2nd Half.xlsx
+++ b/2nd Half.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7620" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7620" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Dividends" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,8 @@
     <sheet name="Weight" sheetId="5" r:id="rId5"/>
     <sheet name="Wealth" sheetId="6" r:id="rId6"/>
     <sheet name="ch12" sheetId="7" r:id="rId7"/>
+    <sheet name="ch26" sheetId="8" r:id="rId8"/>
+    <sheet name="26-11" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="176">
   <si>
     <t xml:space="preserve">Stock Price = </t>
   </si>
@@ -445,6 +447,114 @@
   </si>
   <si>
     <t>WACC</t>
+  </si>
+  <si>
+    <t>Total Current Assets</t>
+  </si>
+  <si>
+    <t>Total Current Liabilities</t>
+  </si>
+  <si>
+    <t>net working capital</t>
+  </si>
+  <si>
+    <t>Inventory</t>
+  </si>
+  <si>
+    <t>COGS</t>
+  </si>
+  <si>
+    <t>COGS in thousands</t>
+  </si>
+  <si>
+    <t>Accounts receivable</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Sales in thousands</t>
+  </si>
+  <si>
+    <t>Accounts Payable</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N = </t>
+  </si>
+  <si>
+    <t>R =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EAR = </t>
+  </si>
+  <si>
+    <t>Daily colletions</t>
+  </si>
+  <si>
+    <t>APR</t>
+  </si>
+  <si>
+    <t>Collection Float</t>
+  </si>
+  <si>
+    <t>Charges</t>
+  </si>
+  <si>
+    <t>Perpetuity</t>
+  </si>
+  <si>
+    <t>Monthly Rate</t>
+  </si>
+  <si>
+    <t>Benefit</t>
+  </si>
+  <si>
+    <t>sales</t>
+  </si>
+  <si>
+    <t>receivables</t>
+  </si>
+  <si>
+    <t>times</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Amount Owed​ ($)</t>
+  </si>
+  <si>
+    <t>Age​ (days)</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>DEF</t>
+  </si>
+  <si>
+    <t>GHI</t>
+  </si>
+  <si>
+    <t>KLM</t>
+  </si>
+  <si>
+    <t>NOP</t>
+  </si>
+  <si>
+    <t>QRS</t>
+  </si>
+  <si>
+    <t>TUV</t>
+  </si>
+  <si>
+    <t>WXY</t>
+  </si>
+  <si>
+    <t>Sum</t>
   </si>
 </sst>
 </file>
@@ -454,12 +564,12 @@
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.0000%"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="171" formatCode="0.00000"/>
-    <numFmt numFmtId="172" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="173" formatCode="0.000%"/>
-    <numFmt numFmtId="174" formatCode="0.00000%"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.000%"/>
+    <numFmt numFmtId="169" formatCode="0.00000%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -487,13 +597,50 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -528,7 +675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -620,18 +767,116 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="172" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2578,7 +2823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -3163,4 +3408,801 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="601" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="38">
+        <v>8157</v>
+      </c>
+      <c r="D1" s="61" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="22">
+        <f>365/(F1-G1)</f>
+        <v>10.735294117647058</v>
+      </c>
+      <c r="F1">
+        <v>45</v>
+      </c>
+      <c r="G1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="39">
+        <v>3535</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" s="60">
+        <f>(B1-B2)*1000</f>
+        <v>4622000</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" s="15">
+        <f>POWER(1+(E2/100), E1) - 1</f>
+        <v>0.19837456531187692</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="38">
+        <v>1496</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="38">
+        <v>4179</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H5" s="38">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="38">
+        <v>13100000</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="38">
+        <v>32700000</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H6" s="38">
+        <v>13100000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="39">
+        <f>B6/1000</f>
+        <v>13100</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" s="39">
+        <f>E6/1000</f>
+        <v>32700</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H7" s="39">
+        <f>H6/1000</f>
+        <v>13100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="5">
+        <f>B5/(B7/365)</f>
+        <v>41.682442748091603</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E8" s="5">
+        <f>E5/(E7/365)</f>
+        <v>46.64633027522936</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H8" s="5">
+        <f>H5/(H7/365)</f>
+        <v>36.63931297709923</v>
+      </c>
+      <c r="J8" s="5">
+        <f>B8+E8-H8</f>
+        <v>51.689460046221733</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>41.682442748091603</v>
+      </c>
+      <c r="E9">
+        <v>30</v>
+      </c>
+      <c r="H9">
+        <v>36.63931297709923</v>
+      </c>
+      <c r="J9" s="5">
+        <f>B9+E9-H9</f>
+        <v>35.043129770992373</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E11" s="38">
+        <v>86000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12">
+        <v>1500</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E12" s="39">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" s="19">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D13" s="46" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13" s="47">
+        <f>(E11/E12)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="3">
+        <v>325</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E14" s="5">
+        <f>365/E13</f>
+        <v>8.4883720930232567</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" s="5">
+        <f>B12*B11</f>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="B16" s="28">
+        <f>B13/12</f>
+        <v>5.8333333333333336E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17" s="5">
+        <f>B14/B16</f>
+        <v>55714.28571428571</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="601" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" style="65" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="62" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="62" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" s="78"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="85" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="86">
+        <v>46000</v>
+      </c>
+      <c r="C2" s="85">
+        <v>36</v>
+      </c>
+      <c r="D2" s="78"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="78"/>
+      <c r="V2" s="78"/>
+      <c r="W2" s="78"/>
+      <c r="X2" s="78"/>
+      <c r="Y2" s="78"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="75">
+        <v>37000</v>
+      </c>
+      <c r="C3" s="74">
+        <v>5</v>
+      </c>
+      <c r="D3" s="78"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="80"/>
+      <c r="P3" s="78"/>
+      <c r="Q3" s="78"/>
+      <c r="R3" s="78"/>
+      <c r="S3" s="78"/>
+      <c r="T3" s="78"/>
+      <c r="U3" s="78"/>
+      <c r="V3" s="78"/>
+      <c r="W3" s="78"/>
+      <c r="X3" s="78"/>
+      <c r="Y3" s="78"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="75">
+        <v>13000</v>
+      </c>
+      <c r="C4" s="74">
+        <v>11</v>
+      </c>
+      <c r="D4" s="78"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="78"/>
+      <c r="Q4" s="78"/>
+      <c r="R4" s="78"/>
+      <c r="S4" s="78"/>
+      <c r="T4" s="78"/>
+      <c r="U4" s="78"/>
+      <c r="V4" s="78"/>
+      <c r="W4" s="78"/>
+      <c r="X4" s="78"/>
+      <c r="Y4" s="78"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="76" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" s="77">
+        <v>77000</v>
+      </c>
+      <c r="C5" s="76">
+        <v>22</v>
+      </c>
+      <c r="D5" s="78"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="83"/>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="78"/>
+      <c r="S5" s="78"/>
+      <c r="T5" s="78"/>
+      <c r="U5" s="78"/>
+      <c r="V5" s="78"/>
+      <c r="W5" s="78"/>
+      <c r="X5" s="78"/>
+      <c r="Y5" s="78"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="85" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" s="86">
+        <v>44000</v>
+      </c>
+      <c r="C6" s="85">
+        <v>40</v>
+      </c>
+      <c r="D6" s="78"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="78"/>
+      <c r="P6" s="78"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="78"/>
+      <c r="S6" s="78"/>
+      <c r="T6" s="78"/>
+      <c r="U6" s="78"/>
+      <c r="V6" s="78"/>
+      <c r="W6" s="78"/>
+      <c r="X6" s="78"/>
+      <c r="Y6" s="78"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="74" t="s">
+        <v>172</v>
+      </c>
+      <c r="B7" s="75">
+        <v>19000</v>
+      </c>
+      <c r="C7" s="74">
+        <v>11</v>
+      </c>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="78"/>
+      <c r="I7" s="78"/>
+      <c r="J7" s="78"/>
+      <c r="K7" s="78"/>
+      <c r="L7" s="78"/>
+      <c r="M7" s="78"/>
+      <c r="N7" s="78"/>
+      <c r="O7" s="78"/>
+      <c r="P7" s="78"/>
+      <c r="Q7" s="78"/>
+      <c r="R7" s="78"/>
+      <c r="S7" s="78"/>
+      <c r="T7" s="78"/>
+      <c r="U7" s="78"/>
+      <c r="V7" s="78"/>
+      <c r="W7" s="78"/>
+      <c r="X7" s="78"/>
+      <c r="Y7" s="78"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="87" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" s="88">
+        <v>77000</v>
+      </c>
+      <c r="C8" s="87">
+        <v>52</v>
+      </c>
+      <c r="D8" s="78"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="78"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="78"/>
+      <c r="L8" s="78"/>
+      <c r="M8" s="78"/>
+      <c r="N8" s="78"/>
+      <c r="O8" s="78"/>
+      <c r="P8" s="78"/>
+      <c r="Q8" s="78"/>
+      <c r="R8" s="78"/>
+      <c r="S8" s="78"/>
+      <c r="T8" s="78"/>
+      <c r="U8" s="78"/>
+      <c r="V8" s="78"/>
+      <c r="W8" s="78"/>
+      <c r="X8" s="78"/>
+      <c r="Y8" s="78"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" s="89" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" s="90">
+        <v>37000</v>
+      </c>
+      <c r="C9" s="89">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="62" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="68">
+        <f>SUM(B2:B9)</f>
+        <v>350000</v>
+      </c>
+      <c r="C10" s="69">
+        <f>SUM(C2:C9)</f>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" s="62" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="62" t="s">
+        <v>166</v>
+      </c>
+      <c r="E12" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="F12" s="62" t="s">
+        <v>165</v>
+      </c>
+      <c r="G12" s="62" t="s">
+        <v>166</v>
+      </c>
+      <c r="I12" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="J12" s="62" t="s">
+        <v>165</v>
+      </c>
+      <c r="K12" s="62" t="s">
+        <v>166</v>
+      </c>
+      <c r="M12" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="N12" s="62" t="s">
+        <v>165</v>
+      </c>
+      <c r="O12" s="62" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q12" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="R12" s="62" t="s">
+        <v>165</v>
+      </c>
+      <c r="S12" s="62" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" s="63" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" s="64">
+        <v>13000</v>
+      </c>
+      <c r="C13" s="63">
+        <v>11</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>170</v>
+      </c>
+      <c r="F13" s="64">
+        <v>77000</v>
+      </c>
+      <c r="G13" s="63">
+        <v>22</v>
+      </c>
+      <c r="I13" s="63" t="s">
+        <v>167</v>
+      </c>
+      <c r="J13" s="64">
+        <v>46000</v>
+      </c>
+      <c r="K13" s="63">
+        <v>36</v>
+      </c>
+      <c r="M13" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="N13" s="64">
+        <v>77000</v>
+      </c>
+      <c r="O13" s="63">
+        <v>52</v>
+      </c>
+      <c r="Q13" s="63" t="s">
+        <v>174</v>
+      </c>
+      <c r="R13" s="64">
+        <v>37000</v>
+      </c>
+      <c r="S13" s="63">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" s="63" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14" s="64">
+        <v>37000</v>
+      </c>
+      <c r="C14" s="63">
+        <v>5</v>
+      </c>
+      <c r="E14" s="71" t="s">
+        <v>175</v>
+      </c>
+      <c r="F14" s="72">
+        <f>SUM(F13:F13)</f>
+        <v>77000</v>
+      </c>
+      <c r="G14" s="73">
+        <f>SUM(G13:G13)</f>
+        <v>22</v>
+      </c>
+      <c r="I14" s="63" t="s">
+        <v>171</v>
+      </c>
+      <c r="J14" s="64">
+        <v>44000</v>
+      </c>
+      <c r="K14" s="63">
+        <v>40</v>
+      </c>
+      <c r="M14" s="71" t="s">
+        <v>175</v>
+      </c>
+      <c r="N14" s="72">
+        <f>SUM(N13:N13)</f>
+        <v>77000</v>
+      </c>
+      <c r="O14" s="73">
+        <f>SUM(O13:O13)</f>
+        <v>52</v>
+      </c>
+      <c r="Q14" s="91" t="s">
+        <v>175</v>
+      </c>
+      <c r="R14" s="92">
+        <f>SUM(R13:R13)</f>
+        <v>37000</v>
+      </c>
+      <c r="S14" s="93">
+        <f>SUM(S13:S13)</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" s="66" t="s">
+        <v>172</v>
+      </c>
+      <c r="B15" s="67">
+        <v>19000</v>
+      </c>
+      <c r="C15" s="66">
+        <v>11</v>
+      </c>
+      <c r="E15" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="84">
+        <f>F14/$B$10</f>
+        <v>0.22</v>
+      </c>
+      <c r="I15" s="71" t="s">
+        <v>175</v>
+      </c>
+      <c r="J15" s="72">
+        <f>SUM(J13:J14)</f>
+        <v>90000</v>
+      </c>
+      <c r="K15" s="73">
+        <f>SUM(K13:K14)</f>
+        <v>76</v>
+      </c>
+      <c r="M15" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="N15" s="84">
+        <f>N14/$B$10</f>
+        <v>0.22</v>
+      </c>
+      <c r="Q15" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="R15" s="84">
+        <f>R14/$B$10</f>
+        <v>0.10571428571428572</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" s="71" t="s">
+        <v>175</v>
+      </c>
+      <c r="B16" s="72">
+        <f>SUM(B13:B15)</f>
+        <v>69000</v>
+      </c>
+      <c r="C16" s="73">
+        <f>SUM(C13:C15)</f>
+        <v>27</v>
+      </c>
+      <c r="I16" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="J16" s="84">
+        <f>J15/$B$10</f>
+        <v>0.25714285714285712</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="84">
+        <f>B16/$B$10</f>
+        <v>0.19714285714285715</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>